<commit_message>
combined all dept curriculum in one UG curr doc. PG is not done yet
</commit_message>
<xml_diff>
--- a/data/UG/CHE-BTech.xlsx
+++ b/data/UG/CHE-BTech.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="curriculum" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="340">
   <si>
     <t xml:space="preserve">Semester</t>
   </si>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">CHxxxx</t>
   </si>
   <si>
-    <t xml:space="preserve">Core Elective Basket: Biological Processes</t>
+    <t xml:space="preserve">Core Elective Basket – Biological Processes</t>
   </si>
   <si>
     <t xml:space="preserve">CY1030</t>
@@ -288,6 +288,9 @@
     <t xml:space="preserve">LA-1/CA-1</t>
   </si>
   <si>
+    <t xml:space="preserve">XXXXXX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Free Elective</t>
   </si>
   <si>
@@ -417,24 +420,24 @@
     <t xml:space="preserve">Can be taken in any semester</t>
   </si>
   <si>
+    <t xml:space="preserve">Course Name (Optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credits (optional)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basket Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Course Name (Optional)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credits (optional)</t>
+    <t xml:space="preserve">CHXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systems Biology</t>
   </si>
   <si>
     <t xml:space="preserve">Biological Processes</t>
   </si>
   <si>
-    <t xml:space="preserve">CHXXXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systems Biology</t>
-  </si>
-  <si>
     <t xml:space="preserve">Drug delivery systems</t>
   </si>
   <si>
@@ -453,15 +456,15 @@
     <t xml:space="preserve">Biomechanics</t>
   </si>
   <si>
+    <t xml:space="preserve">CH6690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Storage Systems</t>
+  </si>
+  <si>
     <t xml:space="preserve">Energy and Environment</t>
   </si>
   <si>
-    <t xml:space="preserve">CH6690</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Storage Systems</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sustainable and Energy Options</t>
   </si>
   <si>
@@ -492,12 +495,12 @@
     <t xml:space="preserve">Air Pollution</t>
   </si>
   <si>
+    <t xml:space="preserve">Engineering Materials</t>
+  </si>
+  <si>
     <t xml:space="preserve">Materials</t>
   </si>
   <si>
-    <t xml:space="preserve">Engineering Materials</t>
-  </si>
-  <si>
     <t xml:space="preserve">Concepts in Soft Matter Systems</t>
   </si>
   <si>
@@ -510,15 +513,15 @@
     <t xml:space="preserve">Interfacial Chemistry</t>
   </si>
   <si>
+    <t xml:space="preserve">CH1480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Technology</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chemical Processes</t>
   </si>
   <si>
-    <t xml:space="preserve">CH1480</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical Technology</t>
-  </si>
-  <si>
     <t xml:space="preserve">CH2580</t>
   </si>
   <si>
@@ -564,19 +567,7 @@
     <t xml:space="preserve">Membrane Separation Process</t>
   </si>
   <si>
-    <t xml:space="preserve">in 5th sem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in 6th sem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in 7th sem</t>
-  </si>
-  <si>
     <t xml:space="preserve">project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in 8th sem</t>
   </si>
   <si>
     <t xml:space="preserve">Elective</t>
@@ -1315,10 +1306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z72"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2330,7 +2321,9 @@
       <c r="D27" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="n">
+        <v>16</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2920,17 +2913,21 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="A43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2958,10 +2955,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D44" s="3" t="n">
         <v>1</v>
@@ -2996,10 +2993,10 @@
         <v>5</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>2</v>
@@ -3034,10 +3031,10 @@
         <v>5</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>1</v>
@@ -3072,10 +3069,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D47" s="3" t="n">
         <v>2</v>
@@ -3110,10 +3107,10 @@
         <v>5</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D48" s="3" t="n">
         <v>1</v>
@@ -3148,10 +3145,10 @@
         <v>5</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D49" s="3" t="n">
         <v>2</v>
@@ -3186,10 +3183,10 @@
         <v>5</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D50" s="3" t="n">
         <v>2</v>
@@ -3224,10 +3221,10 @@
         <v>5</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D51" s="3" t="n">
         <v>1</v>
@@ -3265,7 +3262,7 @@
         <v>57</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D52" s="3" t="n">
         <v>3</v>
@@ -3301,7 +3298,7 @@
         <v>41</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D53" s="3" t="n">
         <v>2</v>
@@ -3330,17 +3327,21 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
+      <c r="A54" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C54" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D54" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3368,10 +3369,10 @@
         <v>6</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D55" s="3" t="n">
         <v>1</v>
@@ -3406,10 +3407,10 @@
         <v>6</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D56" s="3" t="n">
         <v>1</v>
@@ -3444,10 +3445,10 @@
         <v>6</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D57" s="3" t="n">
         <v>1</v>
@@ -3482,10 +3483,10 @@
         <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D58" s="3" t="n">
         <v>1</v>
@@ -3520,10 +3521,10 @@
         <v>6</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D59" s="3" t="n">
         <v>2</v>
@@ -3561,7 +3562,7 @@
         <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D60" s="3" t="n">
         <v>3</v>
@@ -3597,7 +3598,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D61" s="3" t="n">
         <v>2</v>
@@ -3626,17 +3627,21 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+      <c r="A62" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C62" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D62" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3664,10 +3669,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D63" s="3" t="n">
         <v>2</v>
@@ -3702,10 +3707,10 @@
         <v>7</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D64" s="3" t="n">
         <v>1</v>
@@ -3743,7 +3748,7 @@
         <v>41</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="3" t="n">
         <v>2</v>
@@ -3779,7 +3784,7 @@
         <v>57</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D66" s="3" t="n">
         <v>6</v>
@@ -3808,17 +3813,21 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
+      <c r="A67" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C67" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D67" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3846,10 +3855,10 @@
         <v>8</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D68" s="3" t="n">
         <v>2</v>
@@ -3887,7 +3896,7 @@
         <v>41</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D69" s="3" t="n">
         <v>2</v>
@@ -3923,7 +3932,7 @@
         <v>57</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D70" s="3" t="n">
         <v>5</v>
@@ -3952,17 +3961,21 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
+      <c r="A71" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C71" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D71" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -4913,7 +4926,7 @@
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4930,482 +4943,484 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="2" t="n">
+      <c r="E2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="3" t="n">
+      <c r="C3" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="5" t="n">
+      <c r="E3" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="6" t="n">
+      <c r="C8" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="6" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="6" t="n">
+      <c r="E8" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="3" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="6" t="n">
+      <c r="E9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="9" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="6" t="n">
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="6" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" s="5" t="n">
+      <c r="E10" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="6" t="n">
+      <c r="B11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="3" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="5" t="n">
+      <c r="E12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="6" t="n">
+      <c r="C14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="3" t="n">
+      <c r="C15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="E16" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" s="6" t="n">
+      <c r="E22" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="3" t="n">
+      <c r="E23" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="3" t="n">
+      <c r="E24" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="3" t="n">
+      <c r="E25" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B19" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="E26" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B20" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B23" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E23" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B24" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E24" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B25" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E26" s="11" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6399,85 +6414,92 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="D2" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>179</v>
-      </c>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="D3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="D5" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>182</v>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7491,80 +7513,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="D2" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>179</v>
-      </c>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="D3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="D4" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>181</v>
-      </c>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="D5" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>183</v>
-      </c>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8577,310 +8606,313 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="D2" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="n">
+      <c r="E2" s="17" t="n">
         <v>56</v>
       </c>
-      <c r="E2" s="19"/>
       <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="D3" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="n">
+      <c r="E3" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E3" s="19"/>
       <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="D4" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="n">
+      <c r="E4" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E4" s="19"/>
       <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+      <c r="B5" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="D5" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="17" t="n">
+      <c r="E5" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E5" s="19"/>
       <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="B6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="D6" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="17" t="n">
+      <c r="E6" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="19"/>
       <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="B7" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="17" t="n">
+      <c r="E7" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E7" s="19"/>
       <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>115</v>
-      </c>
       <c r="B8" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="E8" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E8" s="19"/>
       <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>99</v>
-      </c>
       <c r="B9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="18" t="n">
+      <c r="C9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="E9" s="17" t="n">
         <v>36</v>
       </c>
-      <c r="E9" s="19"/>
       <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+      <c r="B10" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="F10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>101</v>
-      </c>
       <c r="B11" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="18" t="n">
+      <c r="C11" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="17" t="n">
+      <c r="E11" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E11" s="19"/>
       <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="18" t="n">
+      <c r="D12" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="E12" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="E12" s="19"/>
       <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>95</v>
-      </c>
       <c r="B13" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="18" t="n">
+      <c r="C13" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="17" t="n">
+      <c r="E13" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="E13" s="19"/>
       <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
+      <c r="B14" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="20" t="n">
+      <c r="C14" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="F14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
-        <v>93</v>
-      </c>
       <c r="B15" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="18" t="n">
+      <c r="C15" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="17" t="n">
+      <c r="E15" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="E15" s="19"/>
       <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
-        <v>109</v>
-      </c>
       <c r="B16" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="18" t="n">
+      <c r="C16" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="17" t="n">
+      <c r="E16" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="E16" s="19"/>
       <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="B17" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="18" t="n">
+      <c r="C17" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="17" t="n">
+      <c r="E17" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="E17" s="19"/>
       <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="B18" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C18" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="17" t="n">
+      <c r="E18" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="E18" s="19"/>
       <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9882,7 +9914,7 @@
   </sheetPr>
   <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -9892,7 +9924,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="54.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
@@ -9906,19 +9938,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>189</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>192</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>5</v>
@@ -9946,13 +9978,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D2" s="22" t="n">
         <v>2</v>
@@ -9960,13 +9992,13 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="23" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -9988,7 +10020,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>27</v>
@@ -10002,13 +10034,13 @@
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -10030,7 +10062,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>29</v>
@@ -10044,13 +10076,13 @@
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
       <c r="G4" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -10072,7 +10104,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>9</v>
@@ -10086,13 +10118,13 @@
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -10114,7 +10146,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>31</v>
@@ -10128,13 +10160,13 @@
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -10156,7 +10188,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>11</v>
@@ -10170,13 +10202,13 @@
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -10198,7 +10230,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>33</v>
@@ -10212,13 +10244,13 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -10240,7 +10272,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>35</v>
@@ -10254,13 +10286,13 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -10282,7 +10314,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>51</v>
@@ -10296,13 +10328,13 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -10324,7 +10356,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>53</v>
@@ -10338,13 +10370,13 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -10366,7 +10398,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>71</v>
@@ -10380,13 +10412,13 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -10408,7 +10440,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>73</v>
@@ -10422,13 +10454,13 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -10450,10 +10482,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>56</v>
@@ -10464,13 +10496,13 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -10492,10 +10524,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>76</v>
@@ -10508,13 +10540,13 @@
         <v>34</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -10536,7 +10568,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>77</v>
@@ -10550,13 +10582,13 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -10578,7 +10610,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>79</v>
@@ -10592,13 +10624,13 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -10620,10 +10652,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>82</v>
@@ -10634,13 +10666,13 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -10662,7 +10694,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>83</v>
@@ -10676,13 +10708,13 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -10704,13 +10736,13 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D20" s="22" t="n">
         <v>2</v>
@@ -10718,13 +10750,13 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -10746,13 +10778,13 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D21" s="22" t="n">
         <v>1</v>
@@ -10760,13 +10792,13 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="23" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -10788,13 +10820,13 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="22" t="n">
         <v>1</v>
@@ -10802,13 +10834,13 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -10830,13 +10862,13 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D23" s="22" t="n">
         <v>1</v>
@@ -10844,13 +10876,13 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -10872,13 +10904,13 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D24" s="22" t="n">
         <v>1</v>
@@ -10886,13 +10918,13 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -10914,13 +10946,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="22" t="n">
         <v>2</v>
@@ -10928,13 +10960,13 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -10956,13 +10988,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" s="22" t="n">
         <v>1</v>
@@ -10970,13 +11002,13 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -10998,13 +11030,13 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D27" s="22" t="n">
         <v>1</v>
@@ -11012,13 +11044,13 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -11040,13 +11072,13 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D28" s="22" t="n">
         <v>2</v>
@@ -11054,13 +11086,13 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -11082,13 +11114,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D29" s="22" t="n">
         <v>2</v>
@@ -11096,13 +11128,13 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -11124,13 +11156,13 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" s="22" t="n">
         <v>2</v>
@@ -11138,13 +11170,13 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -11166,13 +11198,13 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D31" s="22" t="n">
         <v>1</v>
@@ -11180,13 +11212,13 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -11208,13 +11240,13 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D32" s="22" t="n">
         <v>2</v>
@@ -11222,13 +11254,13 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -11250,13 +11282,13 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D33" s="22" t="n">
         <v>1</v>
@@ -11264,13 +11296,13 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -11292,13 +11324,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D34" s="22" t="n">
         <v>2</v>
@@ -11306,13 +11338,13 @@
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
       <c r="G34" s="23" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -11334,13 +11366,13 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D35" s="23" t="n">
         <v>1</v>
@@ -11348,7 +11380,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="23" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
@@ -11372,13 +11404,13 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D36" s="22" t="n">
         <v>2</v>
@@ -11386,13 +11418,13 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -11414,13 +11446,13 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D37" s="22" t="n">
         <v>2</v>
@@ -11428,13 +11460,13 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I37" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -11457,10 +11489,10 @@
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="22"/>
       <c r="B38" s="22" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D38" s="22" t="n">
         <v>2</v>
@@ -11468,13 +11500,13 @@
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -11497,10 +11529,10 @@
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="22"/>
       <c r="B39" s="23" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D39" s="23" t="n">
         <v>2</v>
@@ -11508,7 +11540,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
       <c r="G39" s="23" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
@@ -11533,10 +11565,10 @@
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="22"/>
       <c r="B40" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D40" s="22" t="n">
         <v>2</v>
@@ -11544,13 +11576,13 @@
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -11573,10 +11605,10 @@
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="22"/>
       <c r="B41" s="22" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D41" s="22" t="n">
         <v>2</v>
@@ -11584,13 +11616,13 @@
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
       <c r="G41" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -11613,10 +11645,10 @@
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="22"/>
       <c r="B42" s="22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D42" s="23" t="n">
         <v>1</v>
@@ -11624,13 +11656,13 @@
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H42" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -11652,13 +11684,13 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D43" s="22" t="n">
         <v>2</v>
@@ -11666,13 +11698,13 @@
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -11695,10 +11727,10 @@
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="22"/>
       <c r="B44" s="22" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D44" s="23" t="n">
         <v>2</v>
@@ -11706,13 +11738,13 @@
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
       <c r="G44" s="22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -11735,10 +11767,10 @@
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="22"/>
       <c r="B45" s="22" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D45" s="22" t="n">
         <v>2</v>
@@ -11746,13 +11778,13 @@
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
       <c r="G45" s="23" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -11774,13 +11806,13 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D46" s="22" t="n">
         <v>1</v>
@@ -11788,13 +11820,13 @@
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
       <c r="G46" s="22" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -11817,26 +11849,26 @@
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="22"/>
       <c r="B47" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D47" s="22" t="n">
         <v>2</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -11859,10 +11891,10 @@
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="22"/>
       <c r="B48" s="23" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D48" s="23" t="n">
         <v>2</v>
@@ -11870,7 +11902,7 @@
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
       <c r="G48" s="23" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
@@ -11895,10 +11927,10 @@
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="22"/>
       <c r="B49" s="22" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D49" s="22" t="n">
         <v>1</v>
@@ -11906,13 +11938,13 @@
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
       <c r="G49" s="23" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -11935,26 +11967,26 @@
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="22"/>
       <c r="B50" s="22" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D50" s="22" t="n">
         <v>2</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -11976,29 +12008,29 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D51" s="22" t="n">
         <v>2</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -12020,13 +12052,13 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D52" s="22" t="n">
         <v>2</v>
@@ -12034,13 +12066,13 @@
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -12062,13 +12094,13 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D53" s="22" t="n">
         <v>2</v>
@@ -12076,13 +12108,13 @@
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
       <c r="G53" s="22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -12104,13 +12136,13 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D54" s="22" t="n">
         <v>2</v>
@@ -12118,13 +12150,13 @@
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
       <c r="G54" s="23" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -12146,29 +12178,29 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D55" s="22" t="n">
         <v>2</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -12191,10 +12223,10 @@
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="22"/>
       <c r="B56" s="22" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D56" s="22" t="n">
         <v>2</v>
@@ -12202,13 +12234,13 @@
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -12231,10 +12263,10 @@
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="22"/>
       <c r="B57" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D57" s="22" t="n">
         <v>1</v>
@@ -12242,13 +12274,13 @@
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -12271,10 +12303,10 @@
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="22"/>
       <c r="B58" s="22" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D58" s="22" t="n">
         <v>2</v>
@@ -12282,13 +12314,13 @@
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
       <c r="G58" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -12310,13 +12342,13 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D59" s="22" t="n">
         <v>2</v>
@@ -12324,13 +12356,13 @@
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
       <c r="G59" s="23" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H59" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -12352,13 +12384,13 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D60" s="22" t="n">
         <v>2</v>
@@ -12366,13 +12398,13 @@
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H60" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -12394,13 +12426,13 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D61" s="22" t="n">
         <v>2</v>
@@ -12408,13 +12440,13 @@
       <c r="E61" s="22"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -12436,13 +12468,13 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D62" s="22" t="n">
         <v>2</v>
@@ -12450,13 +12482,13 @@
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
       <c r="G62" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H62" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -12478,7 +12510,7 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B63" s="23" t="s">
         <v>162</v>
@@ -12492,13 +12524,13 @@
       <c r="E63" s="22"/>
       <c r="F63" s="22"/>
       <c r="G63" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -12520,13 +12552,13 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D64" s="22" t="n">
         <v>1</v>
@@ -12534,13 +12566,13 @@
       <c r="E64" s="22"/>
       <c r="F64" s="22"/>
       <c r="G64" s="23" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -12562,13 +12594,13 @@
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D65" s="22" t="n">
         <v>1</v>
@@ -12576,13 +12608,13 @@
       <c r="E65" s="22"/>
       <c r="F65" s="22"/>
       <c r="G65" s="22" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H65" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -12604,13 +12636,13 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D66" s="22" t="n">
         <v>1</v>
@@ -12618,13 +12650,13 @@
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
       <c r="G66" s="23" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H66" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -12646,7 +12678,7 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B67" s="23" t="s">
         <v>143</v>
@@ -12660,13 +12692,13 @@
       <c r="E67" s="22"/>
       <c r="F67" s="22"/>
       <c r="G67" s="22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H67" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -12688,13 +12720,13 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D68" s="22" t="n">
         <v>1</v>
@@ -12702,13 +12734,13 @@
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
       <c r="G68" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H68" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -12730,13 +12762,13 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D69" s="22" t="n">
         <v>1</v>
@@ -12744,13 +12776,13 @@
       <c r="E69" s="22"/>
       <c r="F69" s="22"/>
       <c r="G69" s="23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -12772,13 +12804,13 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D70" s="22" t="n">
         <v>1</v>
@@ -12786,13 +12818,13 @@
       <c r="E70" s="22"/>
       <c r="F70" s="22"/>
       <c r="G70" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -12814,13 +12846,13 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D71" s="22" t="n">
         <v>1</v>
@@ -12828,13 +12860,13 @@
       <c r="E71" s="22"/>
       <c r="F71" s="22"/>
       <c r="G71" s="22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H71" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -12856,13 +12888,13 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B72" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D72" s="22" t="n">
         <v>1</v>
@@ -12870,13 +12902,13 @@
       <c r="E72" s="22"/>
       <c r="F72" s="22"/>
       <c r="G72" s="22" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H72" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -12898,13 +12930,13 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D73" s="22" t="n">
         <v>1</v>
@@ -12912,13 +12944,13 @@
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
       <c r="G73" s="22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H73" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -12940,29 +12972,29 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B74" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D74" s="22" t="n">
         <v>2</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G74" s="22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H74" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
@@ -12984,13 +13016,13 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B75" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D75" s="22" t="n">
         <v>1</v>
@@ -12998,13 +13030,13 @@
       <c r="E75" s="22"/>
       <c r="F75" s="22"/>
       <c r="G75" s="22" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H75" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -13030,7 +13062,7 @@
         <v>134</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D76" s="22" t="n">
         <v>2</v>
@@ -13038,13 +13070,13 @@
       <c r="E76" s="22"/>
       <c r="F76" s="22"/>
       <c r="G76" s="22" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H76" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -13066,13 +13098,13 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="22" t="n">
         <v>1</v>
@@ -13080,13 +13112,13 @@
       <c r="E77" s="22"/>
       <c r="F77" s="22"/>
       <c r="G77" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H77" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -13108,13 +13140,13 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B78" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D78" s="22" t="n">
         <v>1</v>
@@ -13122,13 +13154,13 @@
       <c r="E78" s="22"/>
       <c r="F78" s="22"/>
       <c r="G78" s="22" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H78" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -13151,10 +13183,10 @@
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="22"/>
       <c r="B79" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D79" s="23" t="n">
         <v>3</v>
@@ -13162,7 +13194,7 @@
       <c r="E79" s="22"/>
       <c r="F79" s="22"/>
       <c r="G79" s="26" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H79" s="22"/>
       <c r="I79" s="22"/>
@@ -13186,23 +13218,23 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D80" s="23" t="n">
         <v>1</v>
       </c>
       <c r="E80" s="22"/>
       <c r="F80" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G80" s="23" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H80" s="22"/>
       <c r="I80" s="22"/>
@@ -13226,13 +13258,13 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D81" s="23" t="n">
         <v>2</v>
@@ -13240,7 +13272,7 @@
       <c r="E81" s="22"/>
       <c r="F81" s="22"/>
       <c r="G81" s="23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
@@ -13264,13 +13296,13 @@
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D82" s="8" t="n">
         <v>1</v>
@@ -13278,7 +13310,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>

</xml_diff>